<commit_message>
8/2 update after moving apartment
</commit_message>
<xml_diff>
--- a/DailyLog.xlsx
+++ b/DailyLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0db1185575d0d401/Desktop/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC10488D311E513C5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D80D5AA-65D8-49E2-83CC-B8E1ABEE5A8C}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC10488D311E513C5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AEF6AB1-582B-4CA6-99D0-AC058922D768}"/>
   <bookViews>
-    <workbookView xWindow="-10455" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Day</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>208_ImplementTrie</t>
+  </si>
+  <si>
+    <t>415_AddStrings</t>
+  </si>
+  <si>
+    <t>67_AddBinary</t>
   </si>
 </sst>
 </file>
@@ -368,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,6 +436,19 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>44410</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
8/25 morning at home
</commit_message>
<xml_diff>
--- a/DailyLog.xlsx
+++ b/DailyLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackf\OneDrive - Northeastern University\Desktop\leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0db1185575d0d401/Desktop/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BF46CD-028A-4FC7-818A-44FA705D316A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{E2BF46CD-028A-4FC7-818A-44FA705D316A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70E98749-4620-407C-A682-E2AE9BB4A2C2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="3315" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Day</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>287_FindTheDuplicateNumber</t>
+  </si>
+  <si>
+    <t>348_DesignTicTacToe</t>
   </si>
 </sst>
 </file>
@@ -479,20 +482,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +506,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44402</v>
       </c>
@@ -511,7 +514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44404</v>
       </c>
@@ -519,7 +522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44405</v>
       </c>
@@ -527,12 +530,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44406</v>
       </c>
@@ -540,12 +543,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44410</v>
       </c>
@@ -553,12 +556,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44412</v>
       </c>
@@ -566,7 +569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44413</v>
       </c>
@@ -577,7 +580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -585,7 +588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44422</v>
       </c>
@@ -596,7 +599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -604,7 +607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -612,7 +615,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>19</v>
       </c>
@@ -620,7 +623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44423</v>
       </c>
@@ -631,7 +634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44424</v>
       </c>
@@ -642,7 +645,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>25</v>
       </c>
@@ -650,7 +653,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>27</v>
       </c>
@@ -658,7 +661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44425</v>
       </c>
@@ -669,7 +672,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44426</v>
       </c>
@@ -680,7 +683,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>33</v>
       </c>
@@ -688,7 +691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44427</v>
       </c>
@@ -699,7 +702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>35</v>
       </c>
@@ -707,7 +710,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44429</v>
       </c>
@@ -718,7 +721,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>38</v>
       </c>
@@ -726,7 +729,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>39</v>
       </c>
@@ -734,7 +737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44430</v>
       </c>
@@ -745,7 +748,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>41</v>
       </c>
@@ -753,7 +756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44431</v>
       </c>
@@ -764,7 +767,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>43</v>
       </c>
@@ -772,7 +775,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44432</v>
       </c>
@@ -781,6 +784,17 @@
       </c>
       <c r="C33" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>44433</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
10/30 update for check
</commit_message>
<xml_diff>
--- a/DailyLog.xlsx
+++ b/DailyLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0db1185575d0d401/Desktop/leetcode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackf\OneDrive - Northeastern University\Desktop\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{E2BF46CD-028A-4FC7-818A-44FA705D316A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66C8236F-6DD3-4279-B00C-F8AA03D3EB50}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3447B312-6D56-430D-A5FC-44D3984D7E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3690" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -734,14 +734,14 @@
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -752,7 +752,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44402</v>
       </c>
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44404</v>
       </c>
@@ -768,7 +768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44405</v>
       </c>
@@ -776,12 +776,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44406</v>
       </c>
@@ -789,12 +789,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44410</v>
       </c>
@@ -802,12 +802,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44412</v>
       </c>
@@ -815,7 +815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44413</v>
       </c>
@@ -826,7 +826,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -834,7 +834,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44422</v>
       </c>
@@ -845,7 +845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -853,7 +853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -861,7 +861,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>19</v>
       </c>
@@ -869,7 +869,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44423</v>
       </c>
@@ -880,7 +880,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44424</v>
       </c>
@@ -891,7 +891,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>25</v>
       </c>
@@ -899,7 +899,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>27</v>
       </c>
@@ -907,7 +907,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44425</v>
       </c>
@@ -918,7 +918,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44426</v>
       </c>
@@ -929,7 +929,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>33</v>
       </c>
@@ -937,7 +937,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>44427</v>
       </c>
@@ -948,7 +948,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>35</v>
       </c>
@@ -956,7 +956,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44429</v>
       </c>
@@ -967,7 +967,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>38</v>
       </c>
@@ -975,7 +975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>39</v>
       </c>
@@ -983,7 +983,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>44430</v>
       </c>
@@ -994,7 +994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>41</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>44431</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>43</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44432</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44433</v>
       </c>
@@ -1053,18 +1053,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5B335A-F893-4E97-B268-193044B23A23}">
   <dimension ref="A2:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>49</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>50</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>51</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>52</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>53</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>55</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>56</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>57</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>58</v>
       </c>
@@ -1202,12 +1202,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>75</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>76</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>77</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>78</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>79</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>80</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>81</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>82</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>83</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -1330,8 +1330,11 @@
       <c r="C27" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -1345,23 +1348,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>96</v>
       </c>
       <c r="C29" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>97</v>
       </c>
       <c r="C30" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>98</v>
       </c>
@@ -1372,15 +1381,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>99</v>
       </c>
       <c r="C32" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>100</v>
       </c>
@@ -1391,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -1405,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -1419,39 +1431,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>112</v>
       </c>
       <c r="C37" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>113</v>
       </c>
       <c r="C38" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>114</v>
       </c>
       <c r="C39" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>115</v>
       </c>
       <c r="C40" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>116</v>
       </c>

</xml_diff>